<commit_message>
update word and excel
</commit_message>
<xml_diff>
--- a/EyouelKibretProject2.xlsx
+++ b/EyouelKibretProject2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GW\Year 1\DSA\Project 2\GWU-Algorithms-Fall-2025-Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GW\Year 1\DSA\Project2\GWU-Algorithms-Fall-2025-Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436A6F9-BAD2-4D8B-AA7F-8769DCB9F44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34015F37-7AEE-4910-A185-25DBACA5A39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>a</t>
   </si>
@@ -53,23 +53,42 @@
     <t>Experimental</t>
   </si>
   <si>
-    <t>New Theortical</t>
-  </si>
-  <si>
     <t>Scaling factor</t>
   </si>
   <si>
     <t>O(n)</t>
+  </si>
+  <si>
+    <t>log(n,10)</t>
+  </si>
+  <si>
+    <t>log(a,10)</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>log(c,10)</t>
+  </si>
+  <si>
+    <t>New Experimental</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -226,15 +246,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v>Experimental Results</c:v>
+            <c:v>Theoretical</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -245,66 +265,66 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$17</c:f>
+              <c:f>Sheet1!$G$10:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>2.9999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>100000000</c:v>
+                  <c:v>5.9999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$D$17</c:f>
+              <c:f>Sheet1!$H$10:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>1.31130218505859E-5</c:v>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.14917755126953E-4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4652175903320302E-4</c:v>
+                  <c:v>2.9999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2294216156005807E-3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5644950866699205E-2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2084589004516599</c:v>
+                  <c:v>5.9999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.294384956359799</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>187.02897834777801</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -312,20 +332,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D42F-4336-AAA8-2E4CA42D14F9}"/>
+              <c16:uniqueId val="{00000000-C806-4D00-BAE4-CF2B73D2DDC7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>Theoretical Results</c:v>
+            <c:v>Experimental</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -336,66 +356,66 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$17</c:f>
+              <c:f>Sheet1!$G$10:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>2.9999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>100000000</c:v>
+                  <c:v>5.9999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$10:$E$17</c:f>
+              <c:f>Sheet1!$I$10:$I$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.8360000183600002E-5</c:v>
+                  <c:v>0.85383010366128975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8360000183600001E-4</c:v>
+                  <c:v>1.7965144524058962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8360000183600001E-3</c:v>
+                  <c:v>2.712257920930162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8360000183600001E-2</c:v>
+                  <c:v>3.7013018045217136</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.183600001836</c:v>
+                  <c:v>4.7167893671723489</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8360000183600003</c:v>
+                  <c:v>5.8183592034640403</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.3600001836</c:v>
+                  <c:v>6.9206593358632453</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>183.60000183600002</c:v>
+                  <c:v>8.0080362202924746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -403,12 +423,11 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D42F-4336-AAA8-2E4CA42D14F9}"/>
+              <c16:uniqueId val="{00000001-C806-4D00-BAE4-CF2B73D2DDC7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -417,279 +436,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1578406416"/>
-        <c:axId val="1578408816"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$10:$B$17</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10000</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>100000</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1000000</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="0.00E+00">
-                        <c:v>10000000</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="0.00E+00">
-                        <c:v>100000000</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$10:$B$17</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10000</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>100000</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1000000</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="0.00E+00">
-                        <c:v>10000000</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="0.00E+00">
-                        <c:v>100000000</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-D42F-4336-AAA8-2E4CA42D14F9}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:cat>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$10:$B$17</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10000</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>100000</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1000000</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="0.00E+00">
-                        <c:v>10000000</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="0.00E+00">
-                        <c:v>100000000</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$10:$C$17</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="8"/>
-                      <c:pt idx="0">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>100</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1000</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10000</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>100000</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1000000</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="0.00E+00">
-                        <c:v>10000000</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="0.00E+00">
-                        <c:v>100000000</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-D42F-4336-AAA8-2E4CA42D14F9}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:axId val="1490419712"/>
+        <c:axId val="1490420192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1578406416"/>
+        <c:axId val="1490419712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>n</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -727,7 +483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1578408816"/>
+        <c:crossAx val="1490420192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -735,7 +491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1578408816"/>
+        <c:axId val="1490420192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,67 +511,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>(seconds)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -846,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1578406416"/>
+        <c:crossAx val="1490419712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1493,23 +1189,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>324679</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>43070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{036E74ED-E708-9B72-A2CC-0FBFBB7451C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F47A92D5-6273-5CEE-FDCC-48D379AEB7DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1793,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:F23"/>
+  <dimension ref="B6:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,15 +1503,18 @@
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1826,18 +1525,27 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>10</v>
       </c>
@@ -1848,15 +1556,26 @@
         <v>1.31130218505859E-5</v>
       </c>
       <c r="E10" s="1">
-        <f>(F10*C10)</f>
-        <v>1.8360000183600002E-5</v>
-      </c>
-      <c r="F10" s="1">
-        <f>(204/111111110)</f>
-        <v>1.8360000183600002E-6</v>
+        <f>D10*F10</f>
+        <v>7.1421686922311585</v>
+      </c>
+      <c r="F10" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G10">
+        <f>LOG(B10,10)</f>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f>LOG(C10,10)</f>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f>LOG(E10,10)</f>
+        <v>0.85383010366128975</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>100</v>
       </c>
@@ -1867,15 +1586,26 @@
         <v>1.14917755126953E-4</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E17" si="0">(F11*C11)</f>
-        <v>1.8360000183600001E-4</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11:F17" si="1">(204/111111110)</f>
-        <v>1.8360000183600002E-6</v>
+        <f t="shared" ref="E11:E17" si="0">D11*F11</f>
+        <v>62.591369266462266</v>
+      </c>
+      <c r="F11" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G17" si="1">LOG(B11,10)</f>
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H17" si="2">LOG(C11,10)</f>
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I17" si="3">LOG(E11,10)</f>
+        <v>1.7965144524058962</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1000</v>
       </c>
@@ -1887,14 +1617,25 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>1.8360000183600001E-3</v>
-      </c>
-      <c r="F12" s="1">
+        <v>515.534721966505</v>
+      </c>
+      <c r="F12" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="1"/>
-        <v>1.8360000183600002E-6</v>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>2.712257920930162</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10000</v>
       </c>
@@ -1906,14 +1647,25 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>1.8360000183600001E-2</v>
-      </c>
-      <c r="F13" s="1">
+        <v>5026.9180408174734</v>
+      </c>
+      <c r="F13" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="1"/>
-        <v>1.8360000183600002E-6</v>
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>3.7013018045217136</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>100000</v>
       </c>
@@ -1925,14 +1677,25 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0.183600001836</v>
-      </c>
-      <c r="F14" s="1">
+        <v>52094.199295458697</v>
+      </c>
+      <c r="F14" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="1"/>
-        <v>1.8360000183600002E-6</v>
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>4.7167893671723489</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1000000</v>
       </c>
@@ -1944,14 +1707,25 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>1.8360000183600003</v>
-      </c>
-      <c r="F15" s="1">
+        <v>658202.00888846198</v>
+      </c>
+      <c r="F15" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="1"/>
-        <v>1.8360000183600002E-6</v>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>5.8183592034640403</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>10000000</v>
       </c>
@@ -1963,14 +1737,25 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>18.3600001836</v>
-      </c>
-      <c r="F16" s="1">
+        <v>8330274.9470644305</v>
+      </c>
+      <c r="F16" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="1"/>
-        <v>1.8360000183600002E-6</v>
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>6.9206593358632453</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>100000000</v>
       </c>
@@ -1982,14 +1767,25 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>183.60000183600002</v>
-      </c>
-      <c r="F17" s="1">
+        <v>101867634.242964</v>
+      </c>
+      <c r="F17" s="2">
+        <v>544662.30390000006</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="1"/>
-        <v>1.8360000183600002E-6</v>
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>8.0080362202924746</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18">
         <f>SUM(C10:C17)</f>
@@ -2000,8 +1796,11 @@
         <v>203.63777112960778</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>